<commit_message>
Got IYCF unit cost calculations working
</commit_message>
<xml_diff>
--- a/inputs/demo_national_input.xlsx
+++ b/inputs/demo_national_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -5419,7 +5419,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
         <v>187</v>
       </c>
@@ -5428,7 +5428,7 @@
       </c>
       <c r="C2" s="84"/>
     </row>
-    <row r="3" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
         <v>209</v>
       </c>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="C3" s="84"/>
     </row>
-    <row r="4" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="89" t="s">
         <v>58</v>
       </c>
@@ -5446,7 +5446,7 @@
       </c>
       <c r="C4" s="84"/>
     </row>
-    <row r="5" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>137</v>
       </c>
@@ -5455,77 +5455,77 @@
       </c>
       <c r="C5" s="84"/>
     </row>
-    <row r="6" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="89"/>
       <c r="B6" s="90"/>
       <c r="C6" s="90"/>
     </row>
-    <row r="7" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="89"/>
       <c r="B7" s="90"/>
       <c r="C7" s="90"/>
     </row>
-    <row r="8" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="89"/>
       <c r="B8" s="90"/>
       <c r="C8" s="90"/>
     </row>
-    <row r="9" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="90"/>
       <c r="C9" s="90"/>
     </row>
-    <row r="10" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
     </row>
-    <row r="11" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="91"/>
       <c r="B11" s="90"/>
       <c r="C11" s="90"/>
     </row>
-    <row r="12" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="91"/>
       <c r="B12" s="90"/>
       <c r="C12" s="90"/>
     </row>
-    <row r="13" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="91"/>
       <c r="B13" s="90"/>
       <c r="C13" s="90"/>
     </row>
-    <row r="14" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="91"/>
       <c r="B14" s="90"/>
       <c r="C14" s="90"/>
     </row>
-    <row r="15" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="91"/>
       <c r="B15" s="90"/>
       <c r="C15" s="90"/>
     </row>
-    <row r="16" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="91"/>
       <c r="B16" s="90"/>
       <c r="C16" s="90"/>
     </row>
-    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="91"/>
       <c r="B17" s="90"/>
       <c r="C17" s="90"/>
     </row>
-    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="91"/>
       <c r="B18" s="90"/>
       <c r="C18" s="90"/>
     </row>
-    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="89"/>
       <c r="B19" s="90"/>
       <c r="C19" s="90"/>
     </row>
-    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="89"/>
       <c r="B20" s="90"/>
       <c r="C20" s="90"/>
@@ -5560,74 +5560,74 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
     </row>
-    <row r="11" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
     </row>
-    <row r="12" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="48"/>
     </row>
-    <row r="13" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="48"/>
     </row>
-    <row r="14" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
     </row>
-    <row r="15" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="48"/>
     </row>
-    <row r="16" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="48"/>
     </row>
-    <row r="17" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
     </row>
-    <row r="18" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
     </row>
-    <row r="19" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="48"/>
     </row>
   </sheetData>
@@ -9541,7 +9541,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>29</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
         <v>86</v>
       </c>
@@ -9575,7 +9575,7 @@
       <c r="J3" s="138"/>
       <c r="K3" s="138"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
         <v>61</v>
       </c>
@@ -9592,7 +9592,7 @@
       <c r="J4" s="138"/>
       <c r="K4" s="138"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>149</v>
       </c>
@@ -9609,7 +9609,7 @@
       <c r="J5" s="138"/>
       <c r="K5" s="138"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>198</v>
       </c>
@@ -9628,7 +9628,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>63</v>
       </c>
@@ -9647,7 +9647,7 @@
       <c r="J7" s="138"/>
       <c r="K7" s="138"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
         <v>64</v>
       </c>
@@ -9666,7 +9666,7 @@
       <c r="J8" s="138"/>
       <c r="K8" s="138"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>62</v>
       </c>
@@ -9685,7 +9685,7 @@
       <c r="J9" s="138"/>
       <c r="K9" s="138"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>188</v>
       </c>
@@ -9702,7 +9702,7 @@
       <c r="J10" s="138"/>
       <c r="K10" s="138"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
         <v>208</v>
       </c>
@@ -9719,7 +9719,7 @@
       <c r="J11" s="138"/>
       <c r="K11" s="138"/>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>189</v>
       </c>
@@ -9736,7 +9736,7 @@
       <c r="J12" s="138"/>
       <c r="K12" s="138"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>190</v>
       </c>
@@ -9753,7 +9753,7 @@
       <c r="J13" s="138"/>
       <c r="K13" s="138"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="95" t="s">
         <v>187</v>
       </c>
@@ -9772,7 +9772,7 @@
       <c r="J14" s="138"/>
       <c r="K14" s="138"/>
     </row>
-    <row r="15" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="95" t="s">
         <v>209</v>
       </c>
@@ -9791,7 +9791,7 @@
       <c r="J15" s="138"/>
       <c r="K15" s="138"/>
     </row>
-    <row r="16" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
         <v>57</v>
       </c>
@@ -9812,7 +9812,7 @@
       <c r="J16" s="138"/>
       <c r="K16" s="138"/>
     </row>
-    <row r="17" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>47</v>
       </c>
@@ -9829,7 +9829,7 @@
       <c r="J17" s="138"/>
       <c r="K17" s="138"/>
     </row>
-    <row r="18" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>173</v>
       </c>
@@ -9848,7 +9848,7 @@
       <c r="J18" s="138"/>
       <c r="K18" s="138"/>
     </row>
-    <row r="19" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>199</v>
       </c>
@@ -9867,7 +9867,7 @@
       <c r="J19" s="138"/>
       <c r="K19" s="138"/>
     </row>
-    <row r="20" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
         <v>200</v>
       </c>
@@ -9886,7 +9886,7 @@
       <c r="J20" s="138"/>
       <c r="K20" s="138"/>
     </row>
-    <row r="21" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>196</v>
       </c>
@@ -9905,7 +9905,7 @@
       <c r="J21" s="138"/>
       <c r="K21" s="138"/>
     </row>
-    <row r="22" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
         <v>136</v>
       </c>
@@ -9926,7 +9926,7 @@
       <c r="J22" s="138"/>
       <c r="K22" s="138"/>
     </row>
-    <row r="23" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>34</v>
       </c>
@@ -9945,7 +9945,7 @@
       <c r="J23" s="138"/>
       <c r="K23" s="138"/>
     </row>
-    <row r="24" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="52" t="s">
         <v>88</v>
       </c>
@@ -9962,7 +9962,7 @@
       <c r="J24" s="138"/>
       <c r="K24" s="138"/>
     </row>
-    <row r="25" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
         <v>87</v>
       </c>
@@ -9979,7 +9979,7 @@
       <c r="J25" s="138"/>
       <c r="K25" s="138"/>
     </row>
-    <row r="26" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>137</v>
       </c>
@@ -9996,7 +9996,7 @@
       <c r="J26" s="138"/>
       <c r="K26" s="138"/>
     </row>
-    <row r="27" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>59</v>
       </c>
@@ -10015,7 +10015,7 @@
       <c r="J27" s="138"/>
       <c r="K27" s="138"/>
     </row>
-    <row r="28" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>84</v>
       </c>
@@ -10032,7 +10032,7 @@
       <c r="J28" s="138"/>
       <c r="K28" s="138"/>
     </row>
-    <row r="29" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>58</v>
       </c>
@@ -10051,7 +10051,7 @@
       <c r="J29" s="138"/>
       <c r="K29" s="138"/>
     </row>
-    <row r="30" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
         <v>67</v>
       </c>
@@ -10068,7 +10068,7 @@
       <c r="J30" s="138"/>
       <c r="K30" s="138"/>
     </row>
-    <row r="31" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
         <v>28</v>
       </c>
@@ -10087,7 +10087,7 @@
       <c r="J31" s="138"/>
       <c r="K31" s="138"/>
     </row>
-    <row r="32" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>83</v>
       </c>
@@ -10106,7 +10106,7 @@
       <c r="J32" s="138"/>
       <c r="K32" s="138"/>
     </row>
-    <row r="33" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="52" t="s">
         <v>82</v>
       </c>
@@ -10125,7 +10125,7 @@
       <c r="J33" s="138"/>
       <c r="K33" s="138"/>
     </row>
-    <row r="34" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="52" t="s">
         <v>81</v>
       </c>
@@ -10144,7 +10144,7 @@
       <c r="J34" s="138"/>
       <c r="K34" s="138"/>
     </row>
-    <row r="35" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>79</v>
       </c>
@@ -10163,7 +10163,7 @@
       <c r="J35" s="138"/>
       <c r="K35" s="138"/>
     </row>
-    <row r="36" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="52" t="s">
         <v>80</v>
       </c>
@@ -10182,7 +10182,7 @@
       <c r="J36" s="138"/>
       <c r="K36" s="138"/>
     </row>
-    <row r="37" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="52" t="s">
         <v>85</v>
       </c>
@@ -10199,7 +10199,7 @@
       <c r="J37" s="138"/>
       <c r="K37" s="138"/>
     </row>
-    <row r="38" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>60</v>
       </c>
@@ -10287,7 +10287,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -10316,7 +10316,7 @@
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
@@ -10345,7 +10345,7 @@
       <c r="J3" s="138"/>
       <c r="K3" s="138"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>3</v>
       </c>
@@ -10374,7 +10374,7 @@
       <c r="J4" s="138"/>
       <c r="K4" s="138"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>4</v>
       </c>
@@ -10403,7 +10403,7 @@
       <c r="J5" s="138"/>
       <c r="K5" s="138"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>5</v>
       </c>
@@ -10432,7 +10432,7 @@
       <c r="J6" s="138"/>
       <c r="K6" s="138"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>53</v>
       </c>
@@ -10453,7 +10453,7 @@
       <c r="J7" s="138"/>
       <c r="K7" s="138"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>54</v>
       </c>
@@ -10474,7 +10474,7 @@
       <c r="J8" s="138"/>
       <c r="K8" s="138"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>55</v>
       </c>
@@ -10495,7 +10495,7 @@
       <c r="J9" s="138"/>
       <c r="K9" s="138"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>56</v>
       </c>
@@ -10516,7 +10516,7 @@
       <c r="J10" s="138"/>
       <c r="K10" s="138"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>49</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>50</v>
       </c>
@@ -10556,7 +10556,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>51</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>52</v>
       </c>
@@ -11767,7 +11767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="142"/>
       <c r="C3" s="35" t="s">
         <v>175</v>
@@ -11789,7 +11789,7 @@
       </c>
       <c r="J3" s="100"/>
     </row>
-    <row r="4" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="142"/>
       <c r="C4" s="35" t="s">
         <v>174</v>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="J4" s="100"/>
     </row>
-    <row r="5" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="142" t="s">
         <v>1</v>
       </c>
@@ -11835,7 +11835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="142"/>
       <c r="C6" s="35" t="s">
         <v>175</v>
@@ -11856,7 +11856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="142"/>
       <c r="C7" s="35" t="s">
         <v>174</v>
@@ -11877,7 +11877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="142" t="s">
         <v>2</v>
       </c>
@@ -11900,7 +11900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="142"/>
       <c r="C9" s="35" t="s">
         <v>175</v>
@@ -11921,7 +11921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="142"/>
       <c r="C10" s="35" t="s">
         <v>174</v>
@@ -11942,7 +11942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="142" t="s">
         <v>3</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="142"/>
       <c r="C12" s="35" t="s">
         <v>175</v>
@@ -11986,7 +11986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="142"/>
       <c r="C13" s="35" t="s">
         <v>174</v>
@@ -12007,7 +12007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="142" t="s">
         <v>4</v>
       </c>
@@ -12030,7 +12030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="142"/>
       <c r="C15" s="35" t="s">
         <v>175</v>
@@ -12051,7 +12051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="142"/>
       <c r="C16" s="35" t="s">
         <v>174</v>
@@ -12095,7 +12095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" s="137"/>
       <c r="E18" s="137"/>
       <c r="F18" s="137"/>
@@ -12128,7 +12128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="142"/>
       <c r="C20" s="35" t="s">
         <v>175</v>
@@ -12149,7 +12149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="142"/>
       <c r="C21" s="35" t="s">
         <v>174</v>
@@ -12170,7 +12170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="142" t="s">
         <v>1</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="142"/>
       <c r="C23" s="35" t="s">
         <v>175</v>
@@ -12214,7 +12214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="142"/>
       <c r="C24" s="35" t="s">
         <v>174</v>
@@ -12235,7 +12235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="142" t="s">
         <v>2</v>
       </c>
@@ -12258,7 +12258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="142"/>
       <c r="C26" s="35" t="s">
         <v>175</v>
@@ -12279,7 +12279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="142"/>
       <c r="C27" s="35" t="s">
         <v>174</v>
@@ -12300,7 +12300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="142" t="s">
         <v>3</v>
       </c>
@@ -12323,7 +12323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="142"/>
       <c r="C29" s="35" t="s">
         <v>175</v>
@@ -12344,7 +12344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="142"/>
       <c r="C30" s="35" t="s">
         <v>174</v>
@@ -12365,7 +12365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="142" t="s">
         <v>4</v>
       </c>
@@ -12388,7 +12388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="142"/>
       <c r="C32" s="35" t="s">
         <v>175</v>
@@ -12409,7 +12409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="142"/>
       <c r="C33" s="35" t="s">
         <v>174</v>
@@ -12453,7 +12453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D35" s="137"/>
       <c r="E35" s="137"/>
       <c r="F35" s="137"/>
@@ -12486,7 +12486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="142"/>
       <c r="C37" s="35" t="s">
         <v>175</v>
@@ -12507,7 +12507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="142"/>
       <c r="C38" s="35" t="s">
         <v>174</v>
@@ -12528,7 +12528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="142" t="s">
         <v>1</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="142"/>
       <c r="C40" s="35" t="s">
         <v>175</v>
@@ -12572,7 +12572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="142"/>
       <c r="C41" s="35" t="s">
         <v>174</v>
@@ -12593,7 +12593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B42" s="142" t="s">
         <v>2</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="142"/>
       <c r="C43" s="35" t="s">
         <v>175</v>
@@ -12637,7 +12637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="142"/>
       <c r="C44" s="35" t="s">
         <v>174</v>
@@ -12658,7 +12658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="142" t="s">
         <v>3</v>
       </c>
@@ -12681,7 +12681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="142"/>
       <c r="C46" s="35" t="s">
         <v>175</v>
@@ -12702,7 +12702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="142"/>
       <c r="C47" s="35" t="s">
         <v>174</v>
@@ -12723,7 +12723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="142" t="s">
         <v>4</v>
       </c>
@@ -12746,7 +12746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="142"/>
       <c r="C49" s="35" t="s">
         <v>175</v>
@@ -12767,7 +12767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="142"/>
       <c r="C50" s="35" t="s">
         <v>174</v>
@@ -12814,12 +12814,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -12829,6 +12823,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -17563,7 +17563,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="63" t="s">
         <v>67</v>
       </c>
@@ -17594,7 +17594,7 @@
       <c r="F4" s="132"/>
       <c r="G4" s="132"/>
     </row>
-    <row r="5" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="95" t="s">
         <v>183</v>
       </c>
@@ -17671,7 +17671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
         <v>28</v>
       </c>
@@ -17697,7 +17697,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="52" t="s">
         <v>269</v>
       </c>
@@ -17717,7 +17717,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="52" t="s">
         <v>270</v>
       </c>
@@ -17737,7 +17737,7 @@
         <v>0.38507462686567184</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>58</v>
       </c>
@@ -17763,7 +17763,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="52" t="s">
         <v>270</v>
       </c>
@@ -17783,7 +17783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="52" t="s">
         <v>65</v>
       </c>
@@ -17806,7 +17806,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="52" t="s">
         <v>270</v>
       </c>
@@ -17826,7 +17826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>136</v>
       </c>
@@ -17852,7 +17852,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="52" t="s">
         <v>270</v>
       </c>
@@ -17872,7 +17872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="52" t="s">
         <v>65</v>
       </c>
@@ -17895,7 +17895,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
         <v>270</v>
       </c>
@@ -17915,7 +17915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
         <v>61</v>
       </c>
@@ -17941,7 +17941,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="52" t="s">
         <v>270</v>
       </c>
@@ -17962,7 +17962,7 @@
       </c>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="52" t="s">
         <v>65</v>
       </c>
@@ -17986,7 +17986,7 @@
       </c>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
         <v>270</v>
       </c>
@@ -18007,7 +18007,7 @@
       </c>
       <c r="I16" s="36"/>
     </row>
-    <row r="17" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
         <v>62</v>
       </c>
@@ -18034,7 +18034,7 @@
       </c>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
         <v>269</v>
       </c>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
         <v>63</v>
       </c>
@@ -18081,7 +18081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="52" t="s">
         <v>269</v>
       </c>
@@ -18101,7 +18101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
         <v>64</v>
       </c>
@@ -18127,7 +18127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" s="52" t="s">
         <v>269</v>
       </c>
@@ -18147,7 +18147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>79</v>
       </c>
@@ -18173,7 +18173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="52" t="s">
         <v>269</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="52" t="s">
         <v>270</v>
       </c>
@@ -18213,7 +18213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>80</v>
       </c>
@@ -18239,7 +18239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="52" t="s">
         <v>269</v>
       </c>
@@ -18259,7 +18259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="52" t="s">
         <v>270</v>
       </c>
@@ -18279,7 +18279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="52" t="s">
         <v>81</v>
       </c>
@@ -18305,7 +18305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="52" t="s">
         <v>269</v>
       </c>
@@ -18325,7 +18325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="52" t="s">
         <v>270</v>
       </c>
@@ -18345,7 +18345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="52" t="s">
         <v>82</v>
       </c>
@@ -18371,7 +18371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="52" t="s">
         <v>269</v>
       </c>
@@ -18391,7 +18391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="52" t="s">
         <v>270</v>
       </c>
@@ -18411,7 +18411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="52" t="s">
         <v>83</v>
       </c>
@@ -18437,7 +18437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="52" t="s">
         <v>269</v>
       </c>
@@ -18457,7 +18457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="52" t="s">
         <v>270</v>
       </c>
@@ -18477,7 +18477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="52" t="s">
         <v>60</v>
       </c>
@@ -18503,7 +18503,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="52" t="s">
         <v>269</v>
       </c>
@@ -18523,7 +18523,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="52" t="s">
         <v>270</v>
       </c>
@@ -18543,7 +18543,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41" s="52" t="s">
         <v>16</v>
       </c>
@@ -18566,7 +18566,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="52" t="s">
         <v>269</v>
       </c>
@@ -18586,7 +18586,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="52" t="s">
         <v>270</v>
       </c>
@@ -18606,7 +18606,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="52" t="s">
         <v>84</v>
       </c>
@@ -18632,7 +18632,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="52" t="s">
         <v>269</v>
       </c>
@@ -18652,7 +18652,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="52" t="s">
         <v>85</v>
       </c>
@@ -18678,7 +18678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="52" t="s">
         <v>269</v>
       </c>
@@ -18698,7 +18698,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
         <v>196</v>
       </c>
@@ -18724,7 +18724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="52" t="s">
         <v>269</v>
       </c>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="H1" s="99"/>
     </row>
-    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
         <v>86</v>
       </c>
@@ -18817,7 +18817,7 @@
       </c>
       <c r="H2" s="95"/>
     </row>
-    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="35" t="s">
         <v>269</v>
       </c>
@@ -18835,7 +18835,7 @@
       </c>
       <c r="H3" s="133"/>
     </row>
-    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
         <v>87</v>
       </c>
@@ -18859,7 +18859,7 @@
       </c>
       <c r="H4" s="133"/>
     </row>
-    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="C5" s="35" t="s">
         <v>269</v>
@@ -18878,7 +18878,7 @@
       </c>
       <c r="H5" s="95"/>
     </row>
-    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>88</v>
       </c>
@@ -18902,7 +18902,7 @@
       </c>
       <c r="H6" s="95"/>
     </row>
-    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="C7" s="35" t="s">
         <v>269</v>
@@ -19981,7 +19981,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -19998,10 +19998,10 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -20018,10 +20018,10 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -20038,7 +20038,7 @@
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
@@ -20052,7 +20052,7 @@
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
@@ -20066,7 +20066,7 @@
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -20083,7 +20083,7 @@
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
@@ -20097,7 +20097,7 @@
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
@@ -20114,7 +20114,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
@@ -20141,8 +20141,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20184,7 +20184,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="47"/>
       <c r="B3" s="46" t="s">
         <v>1</v>
@@ -20198,7 +20198,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="47"/>
       <c r="B4" s="46" t="s">
         <v>2</v>
@@ -20212,7 +20212,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="46" t="s">
         <v>3</v>
@@ -20226,7 +20226,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="47"/>
       <c r="B6" s="46" t="s">
         <v>4</v>
@@ -20240,7 +20240,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="47"/>
       <c r="B7" s="46" t="s">
         <v>172</v>
@@ -20265,7 +20265,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="47"/>
       <c r="B10" s="46" t="s">
         <v>1</v>
@@ -20277,7 +20277,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="47"/>
       <c r="B11" s="46" t="s">
         <v>2</v>
@@ -20289,7 +20289,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="46" t="s">
         <v>3</v>
@@ -20301,7 +20301,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="46" t="s">
         <v>4</v>
@@ -20313,7 +20313,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="46" t="s">
         <v>172</v>
@@ -20338,7 +20338,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="46" t="s">
         <v>1</v>
@@ -20352,7 +20352,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="46" t="s">
         <v>2</v>
@@ -20366,7 +20366,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="46" t="s">
         <v>3</v>
@@ -20380,7 +20380,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="46" t="s">
         <v>4</v>
@@ -20394,7 +20394,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="46" t="s">
         <v>172</v>
@@ -20480,8 +20480,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update default parameters based on new studies
</commit_message>
<xml_diff>
--- a/inputs/demo_national_input.xlsx
+++ b/inputs/demo_national_input.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="-21132" windowWidth="20736" windowHeight="11760" tabRatio="961"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4790,18 +4790,18 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6328125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="38.6328125" style="16" customWidth="1"/>
-    <col min="3" max="16384" width="14.453125" style="12"/>
+    <col min="1" max="1" width="27.6640625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="16" customWidth="1"/>
+    <col min="3" max="16384" width="14.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>100</v>
       </c>
@@ -4812,14 +4812,14 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>191</v>
       </c>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="7" t="s">
         <v>193</v>
@@ -4828,7 +4828,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>192</v>
@@ -4837,7 +4837,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
@@ -4906,7 +4906,7 @@
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>30</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="32" t="s">
         <v>129</v>
       </c>
@@ -5047,7 +5047,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>135</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
@@ -5251,15 +5251,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.90625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.453125" style="35"/>
+    <col min="2" max="2" width="47.88671875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -5400,13 +5400,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" style="35" customWidth="1"/>
-    <col min="2" max="16384" width="11.453125" style="35"/>
+    <col min="1" max="1" width="30.109375" style="35" customWidth="1"/>
+    <col min="2" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -5498,7 +5498,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -5612,19 +5612,19 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.90625" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
@@ -6186,7 +6186,7 @@
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="11" t="s">
         <v>86</v>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="11" t="s">
         <v>187</v>
@@ -6331,7 +6331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
         <v>208</v>
@@ -6567,7 +6567,7 @@
     <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
         <v>37</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -7326,7 +7326,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
@@ -7364,16 +7364,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="35" customWidth="1"/>
-    <col min="3" max="4" width="11.453125" style="35"/>
-    <col min="5" max="5" width="17.453125" style="35" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="35"/>
+    <col min="1" max="1" width="33.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" style="35" customWidth="1"/>
+    <col min="3" max="4" width="11.44140625" style="35"/>
+    <col min="5" max="5" width="17.44140625" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>163</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>157</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>156</v>
       </c>
@@ -7444,7 +7444,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>155</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
         <v>154</v>
       </c>
@@ -7480,7 +7480,7 @@
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>153</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>152</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="39" t="s">
         <v>151</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>150</v>
       </c>
@@ -7573,20 +7573,20 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" style="55" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" style="55" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="55" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="55" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.08984375" style="55" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="15.36328125" style="55" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="16.90625" style="55" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="16.08984375" style="55"/>
+    <col min="6" max="7" width="13.109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="15.33203125" style="55" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="16.88671875" style="55" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="16.109375" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>33</v>
       </c>
@@ -7633,7 +7633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>31</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="52" t="s">
         <v>149</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="52" t="s">
         <v>173</v>
       </c>
@@ -7768,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="52" t="s">
         <v>198</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="52" t="s">
         <v>199</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="s">
         <v>195</v>
       </c>
@@ -7900,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>136</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="52" t="s">
         <v>137</v>
       </c>
@@ -7988,7 +7988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="52" t="s">
         <v>84</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="52" t="s">
         <v>58</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="52" t="s">
         <v>67</v>
       </c>
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="52" t="s">
         <v>28</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="52" t="s">
         <v>85</v>
       </c>
@@ -8208,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="52" t="s">
         <v>60</v>
       </c>
@@ -8252,7 +8252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="52"/>
       <c r="C16" s="129"/>
       <c r="D16" s="129"/>
@@ -8268,7 +8268,7 @@
       <c r="N16" s="129"/>
       <c r="O16" s="129"/>
     </row>
-    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="56" t="s">
         <v>32</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="56"/>
       <c r="B18" s="52" t="s">
         <v>86</v>
@@ -8360,7 +8360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="90" t="s">
         <v>187</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="90" t="s">
         <v>208</v>
       </c>
@@ -8448,7 +8448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="91" t="s">
         <v>57</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="52" t="s">
         <v>88</v>
       </c>
@@ -8536,7 +8536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="52" t="s">
         <v>87</v>
       </c>
@@ -8580,7 +8580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="52" t="s">
         <v>59</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="52"/>
       <c r="C25" s="129"/>
       <c r="D25" s="129"/>
@@ -8640,7 +8640,7 @@
       <c r="N25" s="129"/>
       <c r="O25" s="129"/>
     </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="56" t="s">
         <v>37</v>
       </c>
@@ -8688,7 +8688,7 @@
       </c>
       <c r="P26" s="92"/>
     </row>
-    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="59" t="s">
         <v>188</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="56"/>
       <c r="B28" s="59" t="s">
         <v>207</v>
@@ -8777,7 +8777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="59" t="s">
         <v>189</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="59" t="s">
         <v>190</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="52"/>
       <c r="C31" s="130"/>
       <c r="D31" s="130"/>
@@ -8881,7 +8881,7 @@
       <c r="N31" s="129"/>
       <c r="O31" s="129"/>
     </row>
-    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="56" t="s">
         <v>35</v>
       </c>
@@ -8928,7 +8928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="52" t="s">
         <v>64</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="52" t="s">
         <v>62</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="52" t="s">
         <v>47</v>
       </c>
@@ -9060,7 +9060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="52" t="s">
         <v>34</v>
       </c>
@@ -9104,7 +9104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="93"/>
       <c r="B37" s="52" t="s">
         <v>83</v>
@@ -9149,7 +9149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="52" t="s">
         <v>82</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="52" t="s">
         <v>81</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" s="93" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="52" t="s">
         <v>79</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="52" t="s">
         <v>80</v>
       </c>
@@ -9342,22 +9342,22 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -10088,22 +10088,22 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.453125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>217</v>
       </c>
@@ -10462,15 +10462,15 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.08984375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="48.109375" style="35" customWidth="1"/>
     <col min="2" max="2" width="15" style="35" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="12.81640625" style="35"/>
+    <col min="3" max="3" width="14.6640625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>218</v>
       </c>
@@ -10496,7 +10496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>219</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="96" t="s">
         <v>172</v>
       </c>
@@ -10857,7 +10857,7 @@
       <c r="G18" s="132"/>
       <c r="H18" s="132"/>
     </row>
-    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>220</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="96" t="s">
         <v>172</v>
       </c>
@@ -11215,7 +11215,7 @@
       <c r="G35" s="132"/>
       <c r="H35" s="132"/>
     </row>
-    <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="97" t="s">
         <v>221</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="13" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="98" t="s">
         <v>172</v>
       </c>
@@ -11569,12 +11569,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11584,6 +11578,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11601,14 +11601,14 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="12" customWidth="1"/>
-    <col min="2" max="9" width="16.90625" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="14.453125" style="12"/>
+    <col min="1" max="1" width="8.44140625" style="12" customWidth="1"/>
+    <col min="2" max="9" width="16.88671875" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="14.44140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -12697,22 +12697,22 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="34.08984375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.90625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="35" customWidth="1"/>
     <col min="5" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="16384" width="16.08984375" style="35"/>
+    <col min="7" max="16384" width="16.109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="100" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="100" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="101"/>
       <c r="C2" s="102" t="s">
         <v>26</v>
@@ -12727,7 +12727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>223</v>
       </c>
@@ -12811,7 +12811,7 @@
       <c r="E8" s="95"/>
       <c r="F8" s="95"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>224</v>
       </c>
@@ -12836,7 +12836,7 @@
       <c r="F10" s="95"/>
       <c r="G10" s="109"/>
     </row>
-    <row r="11" spans="1:7" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="99" t="s">
         <v>225</v>
       </c>
@@ -12846,7 +12846,7 @@
       <c r="F11" s="111"/>
       <c r="G11" s="112"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>226</v>
       </c>
@@ -12910,7 +12910,7 @@
       </c>
       <c r="G15" s="109"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="113"/>
       <c r="C16" s="114"/>
@@ -12919,7 +12919,7 @@
       <c r="F16" s="95"/>
       <c r="G16" s="109"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>230</v>
       </c>
@@ -13073,7 +13073,7 @@
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="113"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="40"/>
     </row>
   </sheetData>
@@ -13094,23 +13094,23 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="26.90625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="35" customWidth="1"/>
-    <col min="4" max="8" width="14.81640625" style="35" customWidth="1"/>
-    <col min="9" max="12" width="15.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="16.90625" style="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="27.21875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="35" customWidth="1"/>
+    <col min="4" max="8" width="14.77734375" style="35" customWidth="1"/>
+    <col min="9" max="12" width="15.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="16.88671875" style="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="118" t="s">
         <v>212</v>
       </c>
@@ -13144,7 +13144,7 @@
       <c r="O2" s="120"/>
       <c r="P2" s="120"/>
     </row>
-    <row r="3" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="40"/>
       <c r="B3" s="35" t="s">
         <v>71</v>
@@ -13577,7 +13577,7 @@
       <c r="O17" s="118"/>
       <c r="P17" s="118"/>
     </row>
-    <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="43" t="s">
         <v>237</v>
       </c>
@@ -13835,12 +13835,12 @@
       <c r="O26" s="118"/>
       <c r="P26" s="118"/>
     </row>
-    <row r="28" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="99" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="121" t="s">
         <v>239</v>
       </c>
@@ -13874,7 +13874,7 @@
       <c r="O29" s="120"/>
       <c r="P29" s="120"/>
     </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="35" t="s">
         <v>71</v>
@@ -14569,12 +14569,12 @@
       <c r="C54" s="43"/>
       <c r="D54" s="43"/>
     </row>
-    <row r="55" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="99" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A56" s="121" t="s">
         <v>70</v>
       </c>
@@ -14602,7 +14602,7 @@
       <c r="O56" s="120"/>
       <c r="P56" s="120"/>
     </row>
-    <row r="57" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="35" t="s">
         <v>38</v>
@@ -14748,12 +14748,12 @@
       <c r="C63" s="43"/>
       <c r="D63" s="43"/>
     </row>
-    <row r="64" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="99" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A65" s="121" t="s">
         <v>24</v>
       </c>
@@ -14787,7 +14787,7 @@
       <c r="O65" s="120"/>
       <c r="P65" s="120"/>
     </row>
-    <row r="66" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="125"/>
       <c r="B66" s="35" t="s">
         <v>73</v>
@@ -15823,12 +15823,12 @@
       <c r="O101" s="118"/>
       <c r="P101" s="118"/>
     </row>
-    <row r="103" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" s="100" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="99" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" s="36" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A104" s="121" t="s">
         <v>71</v>
       </c>
@@ -15862,7 +15862,7 @@
       <c r="O104" s="120"/>
       <c r="P104" s="120"/>
     </row>
-    <row r="105" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="40"/>
       <c r="B105" s="36"/>
       <c r="C105" s="43" t="s">
@@ -15976,7 +15976,7 @@
       <c r="O108" s="118"/>
       <c r="P108" s="118"/>
     </row>
-    <row r="111" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="40"/>
     </row>
   </sheetData>
@@ -15997,24 +15997,24 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="44.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="17.54296875" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" style="35" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="35" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="35" customWidth="1"/>
     <col min="6" max="6" width="15" style="35" customWidth="1"/>
-    <col min="7" max="7" width="13.6328125" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="7" max="7" width="13.6640625" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="125" t="s">
         <v>25</v>
       </c>
@@ -16055,7 +16055,7 @@
         <v>174.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40"/>
       <c r="B4" s="117" t="s">
         <v>251</v>
@@ -16076,7 +16076,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="104" t="s">
         <v>252</v>
       </c>
@@ -16149,12 +16149,12 @@
       <c r="F9" s="117"/>
       <c r="G9" s="117"/>
     </row>
-    <row r="10" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="99" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="104"/>
       <c r="B11" s="113" t="s">
         <v>195</v>
@@ -16175,16 +16175,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="104"/>
       <c r="B12" s="113"/>
     </row>
-    <row r="13" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="99" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="125" t="s">
         <v>239</v>
       </c>
@@ -16207,7 +16207,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="117" t="s">
         <v>256</v>
@@ -16228,7 +16228,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="125" t="s">
         <v>70</v>
       </c>
@@ -16252,12 +16252,12 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:6" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="99" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="56" t="s">
         <v>49</v>
       </c>
@@ -16304,19 +16304,19 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.1796875" style="35" customWidth="1"/>
-    <col min="2" max="6" width="16.08984375" style="35"/>
-    <col min="7" max="7" width="17.1796875" style="35" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="16.08984375" style="35"/>
+    <col min="1" max="1" width="52.21875" style="35" customWidth="1"/>
+    <col min="2" max="6" width="16.109375" style="35"/>
+    <col min="7" max="7" width="17.21875" style="35" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="16.109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>69</v>
       </c>
@@ -16532,10 +16532,10 @@
         <v>259</v>
       </c>
       <c r="C12" s="136">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="D12" s="136">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="E12" s="136">
         <v>0</v>
@@ -16586,15 +16586,15 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.54296875" style="35" customWidth="1"/>
-    <col min="2" max="2" width="58.90625" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" style="35" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="15" width="15" style="35" customWidth="1"/>
-    <col min="16" max="16384" width="12.81640625" style="35"/>
+    <col min="16" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
       <c r="B1" s="40"/>
       <c r="C1" s="103" t="s">
@@ -16637,7 +16637,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>261</v>
       </c>
@@ -17082,7 +17082,7 @@
         <v>0.83</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
         <v>137</v>
       </c>
@@ -17170,7 +17170,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>262</v>
       </c>
@@ -17382,15 +17382,15 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" style="35" customWidth="1"/>
-    <col min="3" max="7" width="15.54296875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="1" max="1" width="21.33203125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" style="35" customWidth="1"/>
+    <col min="3" max="7" width="15.5546875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="40"/>
       <c r="B1" s="119"/>
       <c r="C1" s="40" t="s">
@@ -17409,7 +17409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>263</v>
       </c>
@@ -17434,7 +17434,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>264</v>
       </c>
@@ -17483,20 +17483,20 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" style="52" customWidth="1"/>
-    <col min="2" max="2" width="30.54296875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="24.81640625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" style="52" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" style="52" customWidth="1"/>
     <col min="4" max="4" width="15" style="35" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" style="35" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="35" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="35"/>
-    <col min="8" max="8" width="17.54296875" style="35" customWidth="1"/>
-    <col min="9" max="16384" width="12.81640625" style="35"/>
+    <col min="5" max="5" width="13.6640625" style="35" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" style="35"/>
+    <col min="8" max="8" width="17.5546875" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>69</v>
       </c>
@@ -18613,16 +18613,16 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="35" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" style="35" customWidth="1"/>
-    <col min="4" max="7" width="17.1796875" style="35" customWidth="1"/>
-    <col min="8" max="16384" width="12.81640625" style="35"/>
+    <col min="2" max="2" width="27.44140625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="35" customWidth="1"/>
+    <col min="4" max="7" width="17.21875" style="35" customWidth="1"/>
+    <col min="8" max="16384" width="12.77734375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="119" t="s">
         <v>69</v>
       </c>
@@ -18789,14 +18789,14 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.36328125" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="str">
         <f>"Percentage of deaths in baseline year ("&amp;start_year&amp;") attributable to cause"</f>
         <v>Percentage of deaths in baseline year (2017) attributable to cause</v>
@@ -18807,7 +18807,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="41"/>
     </row>
-    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -18906,7 +18906,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>31</v>
       </c>
@@ -19112,7 +19112,7 @@
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -19228,13 +19228,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>"Percentage of population in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of population in each category in baseline year (2017)</v>
@@ -19655,13 +19655,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1"/>
-    <col min="2" max="7" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="7" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="str">
         <f>"Percentage of children in each category in baseline year ("&amp;start_year&amp;")"</f>
         <v>Percentage of children in each category in baseline year (2017)</v>
@@ -19791,13 +19791,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -19996,15 +19996,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" style="35" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.453125" style="35"/>
+    <col min="2" max="2" width="19.109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
         <v>178</v>
       </c>
@@ -20021,7 +20021,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>173</v>
       </c>
@@ -20100,7 +20100,7 @@
       <c r="D7" s="44"/>
       <c r="E7" s="80"/>
     </row>
-    <row r="9" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>198</v>
       </c>
@@ -20173,7 +20173,7 @@
       <c r="D14" s="44"/>
       <c r="E14" s="80"/>
     </row>
-    <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>199</v>
       </c>
@@ -20272,15 +20272,15 @@
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>164</v>
       </c>
@@ -20294,7 +20294,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
         <v>69</v>
       </c>
@@ -20306,7 +20306,7 @@
       </c>
       <c r="D2" s="80"/>
     </row>
-    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
         <v>185</v>
       </c>
@@ -20331,21 +20331,21 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="56" style="52" customWidth="1"/>
     <col min="2" max="2" width="20" style="36" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="20.08984375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="32.36328125" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="14.453125" style="35"/>
+    <col min="3" max="3" width="20.44140625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="32.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.44140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
It runs for two regions at least
Haven't successfully tested three yet
</commit_message>
<xml_diff>
--- a/inputs/demo_national_input.xlsx
+++ b/inputs/demo_national_input.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="8"/>
+    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Causes of death" sheetId="4" r:id="rId3"/>
     <sheet name="Nutritional status distribution" sheetId="5" r:id="rId4"/>
     <sheet name="Breastfeeding distribution" sheetId="50" r:id="rId5"/>
-    <sheet name="Time trends" sheetId="51" state="hidden" r:id="rId6"/>
+    <sheet name="Time trends" sheetId="51" r:id="rId6"/>
     <sheet name="IYCF packages" sheetId="55" r:id="rId7"/>
     <sheet name="Treatment of SAM" sheetId="60" r:id="rId8"/>
     <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
@@ -90,7 +85,7 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -105,7 +100,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -168,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0">
       <text>
         <r>
           <rPr>
@@ -267,7 +262,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -325,7 +320,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -368,7 +363,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -402,7 +397,7 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -426,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1271,12 +1266,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1584,7 +1579,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2302,7 +2297,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2338,8 +2333,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2349,7 +2344,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2359,16 +2354,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -2401,7 +2396,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2416,7 +2411,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2446,7 +2441,7 @@
     <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2465,28 +2460,28 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2589,7 +2584,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3403,7 +3398,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3460,7 +3455,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3517,7 +3512,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3574,7 +3569,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3631,7 +3626,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3688,7 +3683,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3745,7 +3740,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3802,7 +3797,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3859,7 +3854,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3916,7 +3911,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3973,7 +3968,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4030,7 +4025,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4087,7 +4082,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4144,7 +4139,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4201,7 +4196,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4258,7 +4253,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4315,7 +4310,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4372,7 +4367,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4421,7 +4416,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11569,12 +11564,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11584,6 +11573,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -14574,7 +14569,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="121" t="s">
         <v>70</v>
       </c>
@@ -16304,7 +16299,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16532,10 +16527,10 @@
         <v>259</v>
       </c>
       <c r="C12" s="136">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="D12" s="136">
-        <v>0.23</v>
+        <v>0.08</v>
       </c>
       <c r="E12" s="136">
         <v>0</v>
@@ -19292,23 +19287,23 @@
         <v>118</v>
       </c>
       <c r="C3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
@@ -19403,23 +19398,23 @@
         <v>121</v>
       </c>
       <c r="C9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
@@ -19785,10 +19780,10 @@
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19797,7 +19792,7 @@
     <col min="2" max="2" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>138</v>
       </c>
@@ -19805,41 +19800,59 @@
         <v>145</v>
       </c>
       <c r="C1">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="D1">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="E1">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="F1">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="G1">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="H1">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="I1">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="J1">
-        <v>2017</v>
+        <v>2024</v>
       </c>
       <c r="K1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2025</v>
+      </c>
+      <c r="L1">
+        <v>2026</v>
+      </c>
+      <c r="M1">
+        <v>2027</v>
+      </c>
+      <c r="N1">
+        <v>2028</v>
+      </c>
+      <c r="O1">
+        <v>2029</v>
+      </c>
+      <c r="P1">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="28">
+        <f>(('Nutritional status distribution'!C4+'Nutritional status distribution'!C5)*(1/60)+('Nutritional status distribution'!D4+'Nutritional status distribution'!D5)*(5/60)+('Nutritional status distribution'!E4+'Nutritional status distribution'!E5)*(6/60)+('Nutritional status distribution'!F4+'Nutritional status distribution'!F5)*(12/60)+('Nutritional status distribution'!G4+'Nutritional status distribution'!G5)*(36/60))</f>
+        <v>0.34434320222452625</v>
+      </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
       <c r="F2" s="28"/>
@@ -19848,18 +19861,28 @@
       <c r="I2" s="28"/>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="28">
+        <f>(('Nutritional status distribution'!C10+'Nutritional status distribution'!C11)*(1/60)+('Nutritional status distribution'!D10+'Nutritional status distribution'!D11)*(5/60)+('Nutritional status distribution'!E10+'Nutritional status distribution'!E11)*(6/60)+('Nutritional status distribution'!F10+'Nutritional status distribution'!F11)*(12/60)+('Nutritional status distribution'!G10+'Nutritional status distribution'!G11)*(36/60))</f>
+        <v>4.4702487716765882E-2</v>
+      </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -19867,19 +19890,29 @@
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="28">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="28">
+        <f>'Nutritional status distribution'!C15*(1/60)+'Nutritional status distribution'!D15*(5/60)+'Nutritional status distribution'!E15*(6/60)+'Nutritional status distribution'!F15*(12/60)+'Nutritional status distribution'!G15*(36/60)</f>
+        <v>0.22016400000000003</v>
+      </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
@@ -19888,12 +19921,22 @@
       <c r="I6" s="28"/>
       <c r="J6" s="28"/>
       <c r="K6" s="28"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28">
+        <v>0.17299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="28">
+        <f>('Nutritional status distribution'!H15*('Demographic projections'!C2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!I15*('Demographic projections'!D2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!J15*('Demographic projections'!E2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!K15*('Demographic projections'!F2/SUM('Demographic projections'!C2:F2)))</f>
+        <v>0.18837666072928053</v>
+      </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
@@ -19902,12 +19945,22 @@
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="28">
+        <f>('Nutritional status distribution'!L15*('Demographic projections'!C2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!M15*('Demographic projections'!D2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!N15*('Demographic projections'!E2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!O15*('Demographic projections'!F2/SUM('Demographic projections'!C2:F2)))</f>
+        <v>0.18837666072928053</v>
+      </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
@@ -19916,15 +19969,25 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>142</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="28">
+        <f>('Breastfeeding distribution'!C2*(1/6)+'Breastfeeding distribution'!D2*(5/6))</f>
+        <v>0.50922873745377717</v>
+      </c>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
@@ -19933,12 +19996,22 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="K10" s="28"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="28">
+        <f>(('Breastfeeding distribution'!E2+'Breastfeeding distribution'!E3+'Breastfeeding distribution'!E4)*(6/18)+('Breastfeeding distribution'!F2+'Breastfeeding distribution'!F3+'Breastfeeding distribution'!F4)*(12/18))</f>
+        <v>0.80834605377276669</v>
+      </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28"/>
@@ -19947,15 +20020,25 @@
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="K11" s="28"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="28"/>
+      <c r="C13" s="28">
+        <f>(neonatal_mortality*(1/60)+infant_mortality*(11/60)+U5_mortality*(48/60))/1000</f>
+        <v>6.1899999999999997E-2</v>
+      </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28"/>
@@ -19963,13 +20046,25 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="28">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="28"/>
+      <c r="C14" s="28">
+        <f>maternal_mortality/1000</f>
+        <v>4.0099999999999997E-3</v>
+      </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
@@ -19978,6 +20073,11 @@
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20331,7 +20431,7 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update demo_regions as well
</commit_message>
<xml_diff>
--- a/inputs/demo_national_input.xlsx
+++ b/inputs/demo_national_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5288D05F-3187-4BF1-AD23-0F45F837DCCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="5"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="961" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -85,8 +91,16 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -95,12 +109,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -163,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -226,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -257,12 +271,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -315,12 +329,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -358,12 +372,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -392,12 +406,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -421,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1266,12 +1280,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1579,7 +1593,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2297,7 +2311,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2333,8 +2347,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2344,7 +2358,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2354,16 +2368,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -2396,7 +2410,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2411,7 +2425,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2441,7 +2455,7 @@
     <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2460,28 +2474,28 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2584,7 +2598,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2614,7 +2628,7 @@
   </cellXfs>
   <cellStyles count="728">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="727"/>
+    <cellStyle name="Comma 2" xfId="727" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3338,8 +3352,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -3398,7 +3412,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3455,7 +3469,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3512,7 +3526,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3569,7 +3583,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3626,7 +3640,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3683,7 +3697,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3740,7 +3754,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3797,7 +3811,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3854,7 +3868,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3911,7 +3925,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3968,7 +3982,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4025,7 +4039,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4082,7 +4096,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4139,7 +4153,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4196,7 +4210,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4253,7 +4267,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4310,7 +4324,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4367,7 +4381,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4416,7 +4430,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4779,7 +4793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -5236,7 +5250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5385,7 +5399,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5483,7 +5497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5597,13 +5611,13 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7307,7 +7321,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="8AA2I9UZPCvjoGOxL0MMyqqXoHDNS7n4JtfrsQRho74JNJJKUigxuy0/aEjLs4m9INQV0OZqejhY0qqpkSRx4A==" saltValue="BKXFXqwFrNK8M/n7gCZbMQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="B14:O21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:O21">
     <sortCondition ref="B14:B21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7316,7 +7330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7349,7 +7363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7558,7 +7572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9327,7 +9341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10073,7 +10087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10447,7 +10461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11564,6 +11578,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11573,12 +11593,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11586,7 +11600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -12682,7 +12696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13079,7 +13093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -14569,7 +14583,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A56" s="121" t="s">
         <v>70</v>
       </c>
@@ -15982,7 +15996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -16292,14 +16306,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16375,10 +16389,10 @@
         <v>259</v>
       </c>
       <c r="C4" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D4" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E4" s="136">
         <v>0</v>
@@ -16413,10 +16427,10 @@
         <v>259</v>
       </c>
       <c r="C6" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D6" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E6" s="136">
         <v>0</v>
@@ -16571,14 +16585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17314,37 +17328,37 @@
         <v>1</v>
       </c>
       <c r="E20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="F20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="G20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="H20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="I20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="J20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="K20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="L20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="M20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="N20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="O20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -17367,14 +17381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17417,16 +17431,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="F3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="G3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
@@ -17448,16 +17462,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="F5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="G5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
@@ -17468,14 +17482,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A8" zoomScale="111" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17554,13 +17568,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="G3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="H3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -17574,13 +17588,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="G4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="H4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -17778,13 +17792,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -17798,13 +17812,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="136">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="G14" s="136">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="H14" s="136">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="I14" s="36"/>
     </row>
@@ -17822,13 +17836,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="I15" s="36"/>
     </row>
@@ -17843,13 +17857,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="136">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="G16" s="136">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="H16" s="136">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="I16" s="36"/>
     </row>
@@ -17885,7 +17899,7 @@
         <v>268</v>
       </c>
       <c r="D18" s="136">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E18" s="136">
         <v>0</v>
@@ -17932,7 +17946,7 @@
         <v>268</v>
       </c>
       <c r="D20" s="136">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E20" s="136">
         <v>0</v>
@@ -17978,7 +17992,7 @@
         <v>268</v>
       </c>
       <c r="D22" s="136">
-        <v>0.46</v>
+        <v>0.19</v>
       </c>
       <c r="E22" s="136">
         <v>0</v>
@@ -18417,19 +18431,19 @@
         <v>268</v>
       </c>
       <c r="D42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -18437,19 +18451,19 @@
         <v>269</v>
       </c>
       <c r="D43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="E43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="F43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="G43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="H43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -18483,19 +18497,19 @@
         <v>268</v>
       </c>
       <c r="D45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="E45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="F45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="G45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="H45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -18529,19 +18543,19 @@
         <v>268</v>
       </c>
       <c r="D47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="F47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="G47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="H47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -18558,7 +18572,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="E48" s="136">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F48" s="136">
         <v>0</v>
@@ -18575,10 +18589,10 @@
         <v>268</v>
       </c>
       <c r="D49" s="136">
-        <v>0.51</v>
+        <v>0.88</v>
       </c>
       <c r="E49" s="136">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="F49" s="136">
         <v>0</v>
@@ -18598,14 +18612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18754,16 +18768,16 @@
         <v>268</v>
       </c>
       <c r="D7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="E7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="G7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H7" s="128"/>
     </row>
@@ -18774,7 +18788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19213,7 +19227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19287,23 +19301,23 @@
         <v>118</v>
       </c>
       <c r="C3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
@@ -19398,23 +19412,23 @@
         <v>121</v>
       </c>
       <c r="C9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
@@ -19640,7 +19654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19776,13 +19790,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -20086,7 +20100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20362,7 +20376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20425,7 +20439,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -21098,7 +21112,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="jSdherlZJbZ8Sy1L59bo9v5QauB4K+9LWnSRVPNbXJxTAgxgiv9ErxgnISHZ2apMgabDAJDnLmaWIXWQOwB0iA==" saltValue="GDpAVnNFn9RTLmsUAjB9Mw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="A2:D38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
     <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21107,7 +21121,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Included prevalence of eclampsia and pre-eclampsia in databook to inform appropriate program coverages
</commit_message>
<xml_diff>
--- a/inputs/demo_national_input.xlsx
+++ b/inputs/demo_national_input.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.chadderdon\GitRepos\OptimaRepos\Nutrition\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E26BB8-BE13-412D-808C-7F373E18CAA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -90,8 +91,16 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -100,12 +109,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0" shapeId="0">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -231,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -262,12 +271,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -291,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -320,12 +329,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -363,12 +372,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0" shapeId="0">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -397,12 +406,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -456,7 +465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -1266,12 +1275,18 @@
   </si>
   <si>
     <t>Effectiveness incidence</t>
+  </si>
+  <si>
+    <t>Prevalence of pre-eclampsia</t>
+  </si>
+  <si>
+    <t>Prevalence of eclampsia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2619,7 +2634,7 @@
   </cellXfs>
   <cellStyles count="728">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="727"/>
+    <cellStyle name="Comma 2" xfId="727" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3343,8 +3358,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -4784,14 +4799,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5230,18 +5245,34 @@
         <v>0.42</v>
       </c>
     </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="C60" s="66">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="66">
+        <v>1.4E-2</v>
+      </c>
+    </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection password="CA9F" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P9NuhmWa02gPyfm9FY6sungY5Lbnt4CuTr1169JIAhDutzMh2HsMtr6NVKK2ey6/oS4EwR7d8IAhWWMSyUWUBA==" saltValue="/Kw/mQdPJDQi9KTYoPS0Fg==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5390,7 +5421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5488,7 +5519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5602,13 +5633,13 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -7312,7 +7343,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="8AA2I9UZPCvjoGOxL0MMyqqXoHDNS7n4JtfrsQRho74JNJJKUigxuy0/aEjLs4m9INQV0OZqejhY0qqpkSRx4A==" saltValue="BKXFXqwFrNK8M/n7gCZbMQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="B14:O21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:O21">
     <sortCondition ref="B14:B21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7321,7 +7352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7354,7 +7385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7563,7 +7594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9332,7 +9363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10078,7 +10109,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10452,7 +10483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11569,12 +11600,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11584,6 +11609,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11591,7 +11622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -12687,7 +12718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13084,7 +13115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -15987,7 +16018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -16297,7 +16328,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -16576,7 +16607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -17372,7 +17403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -17473,7 +17504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -18603,7 +18634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -18779,7 +18810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19218,7 +19249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19645,7 +19676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19781,7 +19812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19986,7 +20017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20262,7 +20293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20325,13 +20356,13 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -20998,7 +21029,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="jSdherlZJbZ8Sy1L59bo9v5QauB4K+9LWnSRVPNbXJxTAgxgiv9ErxgnISHZ2apMgabDAJDnLmaWIXWQOwB0iA==" saltValue="GDpAVnNFn9RTLmsUAjB9Mw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="A2:D38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
     <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21007,7 +21038,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>